<commit_message>
Add MCP Server integration with Claude API - Added complete MCP server in backend/mcp_server/ directory - Updated to work with rebuilt simulation engine API - Added Claude API integration with rate limiting and caching - Added comprehensive test files for validation - MCP server bridges natural language questions with simulation data - All API keys removed for security (use ANTHROPIC_API_KEY env var)
</commit_message>
<xml_diff>
--- a/default_data/headcount.xlsx
+++ b/default_data/headcount.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Code\SimpleSim\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Code\SimpleSim\default_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61E537E-3853-45C7-BF6E-6E88737D4935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F39EA-3D94-4DDF-930C-3BAFA62CF601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="37800" windowHeight="15345" xr2:uid="{DBA0B071-99AB-4EAD-BE9F-451F3DA7D2FD}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="22440" windowHeight="13215" xr2:uid="{DBA0B071-99AB-4EAD-BE9F-451F3DA7D2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -215,7 +215,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{617D7DA6-2EDD-4CDD-AC40-BF52828DE0A5}" name="Table1" displayName="Table1" ref="A1:I448" totalsRowShown="0">
-  <autoFilter ref="A1:I448" xr:uid="{617D7DA6-2EDD-4CDD-AC40-BF52828DE0A5}"/>
+  <autoFilter ref="A1:I448" xr:uid="{617D7DA6-2EDD-4CDD-AC40-BF52828DE0A5}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Operations"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I448">
     <sortCondition ref="A1:A448"/>
   </sortState>
@@ -551,16 +557,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24BA17D-51F1-4BF4-BCC4-EA6768E70AE7}">
-  <dimension ref="A1:I447"/>
+  <dimension ref="A1:I448"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
@@ -596,7 +602,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -622,7 +628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -648,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -674,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -700,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -726,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -752,7 +758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -778,7 +784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -804,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -830,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -856,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -882,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -908,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -934,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -960,7 +966,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -986,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1246,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1298,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -1376,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1428,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1454,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -1480,7 +1486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1532,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1584,7 +1590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -1610,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>25</v>
       </c>
@@ -1766,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -1792,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -1870,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>25</v>
       </c>
@@ -1896,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>25</v>
       </c>
@@ -1922,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -1948,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -1974,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -2026,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -2052,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -2078,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>25</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -2130,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>25</v>
       </c>
@@ -2156,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>25</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>25</v>
       </c>
@@ -2208,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>25</v>
       </c>
@@ -2234,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>25</v>
       </c>
@@ -2260,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2286,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>25</v>
       </c>
@@ -2312,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>29</v>
       </c>
@@ -2338,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>29</v>
       </c>
@@ -2364,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>29</v>
       </c>
@@ -2390,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>29</v>
       </c>
@@ -2416,7 +2422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>29</v>
       </c>
@@ -2442,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>29</v>
       </c>
@@ -2468,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -2494,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -2520,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>29</v>
       </c>
@@ -2546,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>29</v>
       </c>
@@ -2572,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>29</v>
       </c>
@@ -2598,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>29</v>
       </c>
@@ -2624,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>29</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>29</v>
       </c>
@@ -2676,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>29</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>29</v>
       </c>
@@ -2728,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>29</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>29</v>
       </c>
@@ -2780,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>29</v>
       </c>
@@ -2806,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -2832,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>29</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>29</v>
       </c>
@@ -2884,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>30</v>
       </c>
@@ -2910,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>30</v>
       </c>
@@ -2936,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>30</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>30</v>
       </c>
@@ -2988,7 +2994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>30</v>
       </c>
@@ -3014,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>30</v>
       </c>
@@ -3040,7 +3046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>30</v>
       </c>
@@ -3066,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>30</v>
       </c>
@@ -3092,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>30</v>
       </c>
@@ -3118,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>30</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>30</v>
       </c>
@@ -3170,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>30</v>
       </c>
@@ -3196,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>30</v>
       </c>
@@ -3222,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>30</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>30</v>
       </c>
@@ -3274,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>30</v>
       </c>
@@ -3404,7 +3410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>30</v>
       </c>
@@ -3430,7 +3436,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>30</v>
       </c>
@@ -3456,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>30</v>
       </c>
@@ -3482,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>30</v>
       </c>
@@ -3508,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>30</v>
       </c>
@@ -3534,7 +3540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>30</v>
       </c>
@@ -3560,7 +3566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>30</v>
       </c>
@@ -3586,7 +3592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>30</v>
       </c>
@@ -3612,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>30</v>
       </c>
@@ -3638,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>30</v>
       </c>
@@ -3664,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>30</v>
       </c>
@@ -3690,7 +3696,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>30</v>
       </c>
@@ -3716,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>30</v>
       </c>
@@ -3742,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>30</v>
       </c>
@@ -3768,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>30</v>
       </c>
@@ -3794,7 +3800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>30</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>30</v>
       </c>
@@ -3846,7 +3852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>30</v>
       </c>
@@ -3872,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>30</v>
       </c>
@@ -3898,7 +3904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>30</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>30</v>
       </c>
@@ -3950,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>30</v>
       </c>
@@ -3976,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>30</v>
       </c>
@@ -4002,7 +4008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>30</v>
       </c>
@@ -4028,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>30</v>
       </c>
@@ -4054,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>30</v>
       </c>
@@ -4080,7 +4086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>32</v>
       </c>
@@ -4106,7 +4112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>32</v>
       </c>
@@ -4132,7 +4138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>32</v>
       </c>
@@ -4158,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>32</v>
       </c>
@@ -4184,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>32</v>
       </c>
@@ -4210,7 +4216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>32</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>32</v>
       </c>
@@ -4262,7 +4268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>32</v>
       </c>
@@ -4288,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>32</v>
       </c>
@@ -4314,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>32</v>
       </c>
@@ -4340,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>32</v>
       </c>
@@ -4366,7 +4372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>32</v>
       </c>
@@ -4392,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>32</v>
       </c>
@@ -4418,7 +4424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>32</v>
       </c>
@@ -4444,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>32</v>
       </c>
@@ -4470,7 +4476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>32</v>
       </c>
@@ -4496,7 +4502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>32</v>
       </c>
@@ -4522,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>32</v>
       </c>
@@ -4548,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>32</v>
       </c>
@@ -4574,7 +4580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>32</v>
       </c>
@@ -4600,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>32</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>32</v>
       </c>
@@ -4652,7 +4658,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>32</v>
       </c>
@@ -4678,7 +4684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>32</v>
       </c>
@@ -4704,7 +4710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>32</v>
       </c>
@@ -4730,7 +4736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>32</v>
       </c>
@@ -4756,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>33</v>
       </c>
@@ -4782,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>33</v>
       </c>
@@ -4808,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>33</v>
       </c>
@@ -4834,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>33</v>
       </c>
@@ -4860,7 +4866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>33</v>
       </c>
@@ -4886,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>33</v>
       </c>
@@ -4912,7 +4918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>33</v>
       </c>
@@ -4938,7 +4944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>33</v>
       </c>
@@ -4964,7 +4970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>33</v>
       </c>
@@ -4990,7 +4996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>33</v>
       </c>
@@ -5016,7 +5022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>33</v>
       </c>
@@ -5042,7 +5048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>33</v>
       </c>
@@ -5068,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>33</v>
       </c>
@@ -5094,7 +5100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>33</v>
       </c>
@@ -5120,7 +5126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>33</v>
       </c>
@@ -5146,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>33</v>
       </c>
@@ -5224,7 +5230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>33</v>
       </c>
@@ -5250,7 +5256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>33</v>
       </c>
@@ -5276,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>33</v>
       </c>
@@ -5302,7 +5308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>33</v>
       </c>
@@ -5328,7 +5334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>33</v>
       </c>
@@ -5354,7 +5360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>33</v>
       </c>
@@ -5380,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>33</v>
       </c>
@@ -5406,7 +5412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>33</v>
       </c>
@@ -5432,7 +5438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>33</v>
       </c>
@@ -5458,7 +5464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>33</v>
       </c>
@@ -5484,7 +5490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>33</v>
       </c>
@@ -5510,7 +5516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>33</v>
       </c>
@@ -5536,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>33</v>
       </c>
@@ -5562,7 +5568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>33</v>
       </c>
@@ -5588,7 +5594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>33</v>
       </c>
@@ -5614,7 +5620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>33</v>
       </c>
@@ -5640,7 +5646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>33</v>
       </c>
@@ -5666,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>33</v>
       </c>
@@ -5692,7 +5698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>33</v>
       </c>
@@ -5718,7 +5724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>33</v>
       </c>
@@ -5744,7 +5750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>33</v>
       </c>
@@ -5770,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>33</v>
       </c>
@@ -5796,7 +5802,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>33</v>
       </c>
@@ -5822,7 +5828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>33</v>
       </c>
@@ -5848,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>34</v>
       </c>
@@ -5874,7 +5880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>34</v>
       </c>
@@ -5900,7 +5906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>34</v>
       </c>
@@ -5926,7 +5932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>34</v>
       </c>
@@ -5952,7 +5958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>34</v>
       </c>
@@ -5978,7 +5984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>34</v>
       </c>
@@ -6004,7 +6010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>34</v>
       </c>
@@ -6030,7 +6036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>34</v>
       </c>
@@ -6056,7 +6062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>34</v>
       </c>
@@ -6082,7 +6088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>34</v>
       </c>
@@ -6108,7 +6114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>34</v>
       </c>
@@ -6134,7 +6140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>34</v>
       </c>
@@ -6160,7 +6166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>34</v>
       </c>
@@ -6186,7 +6192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>34</v>
       </c>
@@ -6212,7 +6218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>34</v>
       </c>
@@ -6238,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>34</v>
       </c>
@@ -6368,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>34</v>
       </c>
@@ -6394,7 +6400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>34</v>
       </c>
@@ -6420,7 +6426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>34</v>
       </c>
@@ -6446,7 +6452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>34</v>
       </c>
@@ -6472,7 +6478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>34</v>
       </c>
@@ -6498,7 +6504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>34</v>
       </c>
@@ -6524,7 +6530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>34</v>
       </c>
@@ -6550,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>34</v>
       </c>
@@ -6576,7 +6582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>34</v>
       </c>
@@ -6602,7 +6608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>34</v>
       </c>
@@ -6628,7 +6634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>34</v>
       </c>
@@ -6654,7 +6660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>34</v>
       </c>
@@ -6680,7 +6686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>34</v>
       </c>
@@ -6706,7 +6712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>34</v>
       </c>
@@ -6732,7 +6738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>34</v>
       </c>
@@ -6758,7 +6764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>34</v>
       </c>
@@ -6784,7 +6790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>34</v>
       </c>
@@ -6810,7 +6816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>34</v>
       </c>
@@ -6836,7 +6842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>34</v>
       </c>
@@ -6862,7 +6868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>34</v>
       </c>
@@ -6888,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>24</v>
       </c>
@@ -6914,7 +6920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>24</v>
       </c>
@@ -6940,7 +6946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>24</v>
       </c>
@@ -6966,7 +6972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>24</v>
       </c>
@@ -6992,7 +6998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>24</v>
       </c>
@@ -7018,7 +7024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>24</v>
       </c>
@@ -7044,7 +7050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>24</v>
       </c>
@@ -7070,7 +7076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>24</v>
       </c>
@@ -7096,7 +7102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>24</v>
       </c>
@@ -7122,7 +7128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>24</v>
       </c>
@@ -7148,7 +7154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>24</v>
       </c>
@@ -7174,7 +7180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>24</v>
       </c>
@@ -7200,7 +7206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>24</v>
       </c>
@@ -7226,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>24</v>
       </c>
@@ -7252,7 +7258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>24</v>
       </c>
@@ -7278,7 +7284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>24</v>
       </c>
@@ -7304,7 +7310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>24</v>
       </c>
@@ -7330,7 +7336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>24</v>
       </c>
@@ -7460,7 +7466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>24</v>
       </c>
@@ -7486,7 +7492,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>24</v>
       </c>
@@ -7512,7 +7518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>24</v>
       </c>
@@ -7538,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>24</v>
       </c>
@@ -7564,7 +7570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>24</v>
       </c>
@@ -7590,7 +7596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>24</v>
       </c>
@@ -7616,7 +7622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>24</v>
       </c>
@@ -7642,7 +7648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>24</v>
       </c>
@@ -7668,7 +7674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>24</v>
       </c>
@@ -7694,7 +7700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>24</v>
       </c>
@@ -7720,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>24</v>
       </c>
@@ -7746,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>24</v>
       </c>
@@ -7772,7 +7778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>24</v>
       </c>
@@ -7798,7 +7804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>24</v>
       </c>
@@ -7824,7 +7830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>24</v>
       </c>
@@ -7850,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>24</v>
       </c>
@@ -7876,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>24</v>
       </c>
@@ -7902,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>24</v>
       </c>
@@ -7928,7 +7934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>24</v>
       </c>
@@ -7954,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>24</v>
       </c>
@@ -7980,7 +7986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>24</v>
       </c>
@@ -8006,7 +8012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>24</v>
       </c>
@@ -8032,7 +8038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>24</v>
       </c>
@@ -8058,7 +8064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>24</v>
       </c>
@@ -8084,7 +8090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>24</v>
       </c>
@@ -8110,7 +8116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>24</v>
       </c>
@@ -8136,7 +8142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>24</v>
       </c>
@@ -8162,7 +8168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>24</v>
       </c>
@@ -8188,7 +8194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>24</v>
       </c>
@@ -8214,7 +8220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>24</v>
       </c>
@@ -8240,7 +8246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>24</v>
       </c>
@@ -8266,7 +8272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>24</v>
       </c>
@@ -8292,7 +8298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>24</v>
       </c>
@@ -8318,7 +8324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>24</v>
       </c>
@@ -8344,7 +8350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>24</v>
       </c>
@@ -8370,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>24</v>
       </c>
@@ -8396,7 +8402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>22</v>
       </c>
@@ -8422,7 +8428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>22</v>
       </c>
@@ -8448,7 +8454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>22</v>
       </c>
@@ -8474,7 +8480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>22</v>
       </c>
@@ -8500,7 +8506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>22</v>
       </c>
@@ -8526,7 +8532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>22</v>
       </c>
@@ -8552,7 +8558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>22</v>
       </c>
@@ -8578,7 +8584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>22</v>
       </c>
@@ -8604,7 +8610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>22</v>
       </c>
@@ -8630,7 +8636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>22</v>
       </c>
@@ -8656,7 +8662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>22</v>
       </c>
@@ -8682,7 +8688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>22</v>
       </c>
@@ -8708,7 +8714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>22</v>
       </c>
@@ -8734,7 +8740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>22</v>
       </c>
@@ -8760,7 +8766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>22</v>
       </c>
@@ -8786,7 +8792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>22</v>
       </c>
@@ -8916,7 +8922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>22</v>
       </c>
@@ -8942,7 +8948,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>22</v>
       </c>
@@ -8968,7 +8974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>22</v>
       </c>
@@ -8994,7 +9000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>22</v>
       </c>
@@ -9020,7 +9026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>22</v>
       </c>
@@ -9046,7 +9052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>22</v>
       </c>
@@ -9072,7 +9078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>22</v>
       </c>
@@ -9098,7 +9104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>22</v>
       </c>
@@ -9124,7 +9130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>22</v>
       </c>
@@ -9150,7 +9156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>22</v>
       </c>
@@ -9176,7 +9182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>22</v>
       </c>
@@ -9202,7 +9208,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>22</v>
       </c>
@@ -9228,7 +9234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>22</v>
       </c>
@@ -9254,7 +9260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>22</v>
       </c>
@@ -9280,7 +9286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>22</v>
       </c>
@@ -9306,7 +9312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>22</v>
       </c>
@@ -9332,7 +9338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>22</v>
       </c>
@@ -9358,7 +9364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>22</v>
       </c>
@@ -9384,7 +9390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>22</v>
       </c>
@@ -9410,7 +9416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>22</v>
       </c>
@@ -9436,7 +9442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>22</v>
       </c>
@@ -9462,7 +9468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>22</v>
       </c>
@@ -9488,7 +9494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>36</v>
       </c>
@@ -9514,7 +9520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>36</v>
       </c>
@@ -9540,7 +9546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>36</v>
       </c>
@@ -9566,7 +9572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>36</v>
       </c>
@@ -9592,7 +9598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>36</v>
       </c>
@@ -9618,7 +9624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>36</v>
       </c>
@@ -9644,7 +9650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>36</v>
       </c>
@@ -9670,7 +9676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>36</v>
       </c>
@@ -9696,7 +9702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>36</v>
       </c>
@@ -9722,7 +9728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>36</v>
       </c>
@@ -9748,7 +9754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>36</v>
       </c>
@@ -9774,7 +9780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>36</v>
       </c>
@@ -9800,7 +9806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>36</v>
       </c>
@@ -9826,7 +9832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>36</v>
       </c>
@@ -9852,7 +9858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>36</v>
       </c>
@@ -9878,7 +9884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>36</v>
       </c>
@@ -9904,7 +9910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>36</v>
       </c>
@@ -9930,7 +9936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>36</v>
       </c>
@@ -9956,7 +9962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>36</v>
       </c>
@@ -9982,7 +9988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>36</v>
       </c>
@@ -10112,7 +10118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>36</v>
       </c>
@@ -10138,7 +10144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>36</v>
       </c>
@@ -10164,7 +10170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>36</v>
       </c>
@@ -10190,7 +10196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>36</v>
       </c>
@@ -10216,7 +10222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>36</v>
       </c>
@@ -10242,7 +10248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>36</v>
       </c>
@@ -10268,7 +10274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>36</v>
       </c>
@@ -10294,7 +10300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>36</v>
       </c>
@@ -10320,7 +10326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>36</v>
       </c>
@@ -10346,7 +10352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>36</v>
       </c>
@@ -10372,7 +10378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>36</v>
       </c>
@@ -10398,7 +10404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>36</v>
       </c>
@@ -10424,7 +10430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>36</v>
       </c>
@@ -10450,7 +10456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>36</v>
       </c>
@@ -10476,7 +10482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>36</v>
       </c>
@@ -10502,7 +10508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>36</v>
       </c>
@@ -10528,7 +10534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>36</v>
       </c>
@@ -10554,7 +10560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>36</v>
       </c>
@@ -10580,7 +10586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>36</v>
       </c>
@@ -10606,7 +10612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>36</v>
       </c>
@@ -10632,7 +10638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>36</v>
       </c>
@@ -10658,7 +10664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>36</v>
       </c>
@@ -10684,7 +10690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>36</v>
       </c>
@@ -10710,7 +10716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>36</v>
       </c>
@@ -10736,7 +10742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>36</v>
       </c>
@@ -10762,7 +10768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>36</v>
       </c>
@@ -10788,7 +10794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>36</v>
       </c>
@@ -10814,7 +10820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>36</v>
       </c>
@@ -10840,7 +10846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>36</v>
       </c>
@@ -10866,7 +10872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>36</v>
       </c>
@@ -10892,7 +10898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>36</v>
       </c>
@@ -10918,7 +10924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>36</v>
       </c>
@@ -10944,7 +10950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>36</v>
       </c>
@@ -10970,7 +10976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>36</v>
       </c>
@@ -10996,7 +11002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>36</v>
       </c>
@@ -11022,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>36</v>
       </c>
@@ -11048,7 +11054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>38</v>
       </c>
@@ -11074,7 +11080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>38</v>
       </c>
@@ -11100,7 +11106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>38</v>
       </c>
@@ -11126,7 +11132,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>38</v>
       </c>
@@ -11152,7 +11158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>38</v>
       </c>
@@ -11178,7 +11184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>38</v>
       </c>
@@ -11204,7 +11210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>38</v>
       </c>
@@ -11230,7 +11236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>38</v>
       </c>
@@ -11256,7 +11262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>38</v>
       </c>
@@ -11282,7 +11288,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>38</v>
       </c>
@@ -11308,7 +11314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>38</v>
       </c>
@@ -11334,7 +11340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>38</v>
       </c>
@@ -11360,7 +11366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>38</v>
       </c>
@@ -11386,7 +11392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>38</v>
       </c>
@@ -11412,7 +11418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>38</v>
       </c>
@@ -11438,7 +11444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>38</v>
       </c>
@@ -11464,7 +11470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>38</v>
       </c>
@@ -11490,7 +11496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>38</v>
       </c>
@@ -11516,7 +11522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>39</v>
       </c>
@@ -11542,7 +11548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>39</v>
       </c>
@@ -11568,7 +11574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>39</v>
       </c>
@@ -11594,7 +11600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>39</v>
       </c>
@@ -11620,7 +11626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>39</v>
       </c>
@@ -11646,7 +11652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>39</v>
       </c>
@@ -11672,7 +11678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>39</v>
       </c>
@@ -11698,7 +11704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>39</v>
       </c>
@@ -11724,7 +11730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>39</v>
       </c>
@@ -11750,7 +11756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>39</v>
       </c>
@@ -11776,7 +11782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>39</v>
       </c>
@@ -11802,7 +11808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>39</v>
       </c>
@@ -11828,7 +11834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>39</v>
       </c>
@@ -11854,7 +11860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>39</v>
       </c>
@@ -11932,7 +11938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>39</v>
       </c>
@@ -11958,7 +11964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>39</v>
       </c>
@@ -11984,7 +11990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>39</v>
       </c>
@@ -12010,7 +12016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>39</v>
       </c>
@@ -12036,7 +12042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>39</v>
       </c>
@@ -12062,7 +12068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>39</v>
       </c>
@@ -12088,7 +12094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>39</v>
       </c>
@@ -12114,7 +12120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>39</v>
       </c>
@@ -12140,7 +12146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>39</v>
       </c>
@@ -12166,7 +12172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>39</v>
       </c>
@@ -12192,6 +12198,7 @@
         <v>0</v>
       </c>
     </row>
+    <row r="448" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>